<commit_message>
Spring Mass Damper SIMULINK
</commit_message>
<xml_diff>
--- a/TunedmassFreqRep.xlsx
+++ b/TunedmassFreqRep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\MATLAB\DVProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF5F1B3B-F83D-4116-91CA-E203DC3EED98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498CFF14-E2E7-4973-86DB-848055B55D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4109D2C6-3F58-4593-B57D-A55CA72EADC5}"/>
   </bookViews>
@@ -195,7 +195,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -218,158 +218,161 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$54</c:f>
+              <c:f>Sheet1!$G$3:$G$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.16</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.24</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.32</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.48</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.55999999999999994</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.64</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.72</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.8</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>0.88000000000000012</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>0.96</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>1.04</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>1.1199999999999999</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1.2</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>1.28</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>1.3599999999999999</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>1.44</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>1.52</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>1.6</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>1.6800000000000002</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>1.7600000000000002</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>1.8399999999999999</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>1.92</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>2.08</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>2.16</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>2.2399999999999998</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>2.3199999999999998</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>2.4</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>2.48</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>2.56</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>2.6399999999999997</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>2.7199999999999998</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>2.8</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>2.88</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>2.96</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>3.04</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>3.12</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>3.2</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>3.28</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>3.3600000000000003</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>3.44</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>3.5200000000000005</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>3.6</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>3.6799999999999997</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>3.7600000000000002</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>3.84</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>3.9200000000000004</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -377,158 +380,161 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$54</c:f>
+              <c:f>Sheet1!$H$3:$H$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="53"/>
+                <c:ptCount val="54"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>8.719063310663959E-3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3.8536470217955782E-2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>9.7462537462537469E-2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.19921449495497462</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.36949152542372887</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.66339418037231146</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.2271623428724254</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2.6352572268495851</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>12.168295687885012</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>-6.9714285714285582</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>-2.8817025538307428</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>-1.6704203461674321</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>-0.85489936917993348</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>2.5047923322681843E-2</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>1.3679999999999992</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>4.2729007305543645</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>17.311128871128826</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>-29.616692563818006</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>-11.170248030347238</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>-7.9094339622641456</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>-6.577145025135156</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>-5.8719443167640648</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>-5.4494833823742228</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>-5.1790471269882268</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>-4.9999999999999991</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>-4.8803097646258173</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>-4.8014277174646631</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>-4.7518514824407587</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>-4.7240588850979384</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>-4.7129172714078367</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>-4.7148007168387016</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>-4.7270725656938435</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>-4.7477680633580039</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>-4.775392140395196</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>-4.8087862993298582</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>-4.8470384862465687</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>-4.8894205468835441</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>-4.9353438741601483</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>-4.9843273453402173</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>-5.0359737417943107</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>-5.0899521372638308</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>-5.1459845590136819</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>-5.2038357563202853</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>-5.2633052611542377</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>-5.3242211619421829</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>-5.3864351730093416</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>-5.4498186948556508</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>-5.5142596398885591</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>-5.5796598550984688</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="50">
                   <c:v>-5.6459330143540676</c:v>
                 </c:pt>
               </c:numCache>
@@ -1288,16 +1294,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>441739</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>519043</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>115956</xdr:rowOff>
+      <xdr:rowOff>149087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>414131</xdr:colOff>
+      <xdr:colOff>557694</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>93869</xdr:rowOff>
+      <xdr:rowOff>93870</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1622,10 +1628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77ED59E-E113-4603-82DF-3A64DB820D21}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H1" activeCellId="1" sqref="G1:G1048576 H1:H1048576"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1633,61 +1639,30 @@
     <col min="8" max="8" width="15.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1.25</v>
-      </c>
-      <c r="B2">
-        <f>A2</f>
-        <v>1.25</v>
-      </c>
-      <c r="C2">
-        <v>0.1</v>
-      </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E51" si="0">D2*B2/A2</f>
-        <v>0.2</v>
-      </c>
-      <c r="F2">
-        <f>C2/B2</f>
-        <v>0.08</v>
-      </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G51" si="1">C2/A2</f>
-        <v>0.08</v>
-      </c>
-      <c r="H2">
-        <f t="shared" ref="H2:H51" si="2">(C2^2)*((1/A2^2)*(1-F2^2)+1/B2*(E2)) / ((1-F2^2)*(1+E2-G2)-E2)</f>
-        <v>8.719063310663959E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1695,30 +1670,26 @@
         <v>1.25</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B51" si="3">A3</f>
         <v>1.25</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0.2</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F51" si="4">C3/B3</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <f t="shared" si="1"/>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" si="2"/>
-        <v>3.8536470217955782E-2</v>
+        <f t="shared" ref="H3:H53" si="0">(C3^2)*((1/A3^2)*(1-F3^2)+1/B3*(E3)) / ((1-F3^2)*(1+E3-G3)-E3)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1726,30 +1697,30 @@
         <v>1.25</v>
       </c>
       <c r="B4">
-        <f t="shared" si="3"/>
+        <f>A4</f>
         <v>1.25</v>
       </c>
       <c r="C4">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
         <v>0.2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E53" si="1">D4*B4/A4</f>
         <v>0.2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="4"/>
-        <v>0.24</v>
+        <f>C4/B4</f>
+        <v>0.08</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>0.24</v>
+        <f t="shared" ref="G4:G53" si="2">C4/A4</f>
+        <v>0.08</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
-        <v>9.7462537462537469E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.719063310663959E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1757,30 +1728,30 @@
         <v>1.25</v>
       </c>
       <c r="B5">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B5:B53" si="3">A5</f>
         <v>1.25</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D5">
         <v>0.2</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="4"/>
-        <v>0.32</v>
+        <f t="shared" ref="F5:F53" si="4">C5/B5</f>
+        <v>0.16</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>0.32</v>
+        <f t="shared" si="2"/>
+        <v>0.16</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
-        <v>0.19921449495497462</v>
+        <f t="shared" si="0"/>
+        <v>3.8536470217955782E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1792,26 +1763,26 @@
         <v>1.25</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D6">
         <v>0.2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f t="shared" si="2"/>
+        <v>0.24</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
-        <v>0.36949152542372887</v>
+        <f t="shared" si="0"/>
+        <v>9.7462537462537469E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1823,26 +1794,26 @@
         <v>1.25</v>
       </c>
       <c r="C7">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
         <v>0.2</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>0.48</v>
+        <v>0.32</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
+        <f t="shared" si="2"/>
+        <v>0.32</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>0.66339418037231146</v>
+        <f t="shared" si="0"/>
+        <v>0.19921449495497462</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1854,26 +1825,26 @@
         <v>1.25</v>
       </c>
       <c r="C8">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
         <v>0.2</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>0.55999999999999994</v>
+        <v>0.4</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
-        <v>0.55999999999999994</v>
+        <f t="shared" si="2"/>
+        <v>0.4</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
-        <v>1.2271623428724254</v>
+        <f t="shared" si="0"/>
+        <v>0.36949152542372887</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1885,26 +1856,26 @@
         <v>1.25</v>
       </c>
       <c r="C9">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D9">
         <v>0.2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>0.64</v>
+        <v>0.48</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>0.64</v>
+        <f t="shared" si="2"/>
+        <v>0.48</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>2.6352572268495851</v>
+        <f t="shared" si="0"/>
+        <v>0.66339418037231146</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1916,26 +1887,26 @@
         <v>1.25</v>
       </c>
       <c r="C10">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="D10">
         <v>0.2</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F10">
         <f t="shared" si="4"/>
-        <v>0.72</v>
+        <v>0.55999999999999994</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
+        <f t="shared" si="2"/>
+        <v>0.55999999999999994</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>12.168295687885012</v>
+        <f t="shared" si="0"/>
+        <v>1.2271623428724254</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1947,26 +1918,26 @@
         <v>1.25</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
         <v>0.2</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F11">
         <f t="shared" si="4"/>
-        <v>0.8</v>
+        <v>0.64</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="2"/>
+        <v>0.64</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>-6.9714285714285582</v>
+        <f t="shared" si="0"/>
+        <v>2.6352572268495851</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1978,26 +1949,26 @@
         <v>1.25</v>
       </c>
       <c r="C12">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="D12">
         <v>0.2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F12">
         <f t="shared" si="4"/>
-        <v>0.88000000000000012</v>
+        <v>0.72</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>0.88000000000000012</v>
+        <f t="shared" si="2"/>
+        <v>0.72</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>-2.8817025538307428</v>
+        <f t="shared" si="0"/>
+        <v>12.168295687885012</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -2009,26 +1980,26 @@
         <v>1.25</v>
       </c>
       <c r="C13">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0.2</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
-        <v>0.96</v>
+        <f t="shared" si="2"/>
+        <v>0.8</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>-1.6704203461674321</v>
+        <f t="shared" si="0"/>
+        <v>-6.9714285714285582</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -2040,26 +2011,26 @@
         <v>1.25</v>
       </c>
       <c r="C14">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14">
         <v>0.2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
-        <v>1.04</v>
+        <v>0.88000000000000012</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
-        <v>1.04</v>
+        <f t="shared" si="2"/>
+        <v>0.88000000000000012</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
-        <v>-0.85489936917993348</v>
+        <f t="shared" si="0"/>
+        <v>-2.8817025538307428</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -2071,26 +2042,26 @@
         <v>1.25</v>
       </c>
       <c r="C15">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="D15">
         <v>0.2</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>1.1199999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>1.1199999999999999</v>
+        <f t="shared" si="2"/>
+        <v>0.96</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
-        <v>2.5047923322681843E-2</v>
+        <f t="shared" si="0"/>
+        <v>-1.6704203461674321</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -2102,26 +2073,26 @@
         <v>1.25</v>
       </c>
       <c r="C16">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D16">
         <v>0.2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>1.2</v>
+        <v>1.04</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
-        <v>1.2</v>
+        <f t="shared" si="2"/>
+        <v>1.04</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
-        <v>1.3679999999999992</v>
+        <f t="shared" si="0"/>
+        <v>-0.85489936917993348</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -2133,26 +2104,26 @@
         <v>1.25</v>
       </c>
       <c r="C17">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="D17">
         <v>0.2</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
-        <v>1.28</v>
+        <v>1.1199999999999999</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
-        <v>1.28</v>
+        <f t="shared" si="2"/>
+        <v>1.1199999999999999</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
-        <v>4.2729007305543645</v>
+        <f t="shared" si="0"/>
+        <v>2.5047923322681843E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2164,26 +2135,26 @@
         <v>1.25</v>
       </c>
       <c r="C18">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="D18">
         <v>0.2</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>1.3599999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
-        <v>1.3599999999999999</v>
+        <f t="shared" si="2"/>
+        <v>1.2</v>
       </c>
       <c r="H18">
-        <f>(C18^2)*((1/A18^2)*(1-F18^2)+1/B18*(E18)) / ((1-F18^2)*(1+E18-G18)-E18)</f>
-        <v>17.311128871128826</v>
+        <f t="shared" si="0"/>
+        <v>1.3679999999999992</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -2195,26 +2166,26 @@
         <v>1.25</v>
       </c>
       <c r="C19">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="D19">
         <v>0.2</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F19">
         <f t="shared" si="4"/>
-        <v>1.44</v>
+        <v>1.28</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
-        <v>1.44</v>
+        <f t="shared" si="2"/>
+        <v>1.28</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
-        <v>-29.616692563818006</v>
+        <f t="shared" si="0"/>
+        <v>4.2729007305543645</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -2226,26 +2197,26 @@
         <v>1.25</v>
       </c>
       <c r="C20">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="D20">
         <v>0.2</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>1.52</v>
+        <v>1.3599999999999999</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
-        <v>1.52</v>
+        <f t="shared" si="2"/>
+        <v>1.3599999999999999</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
-        <v>-11.170248030347238</v>
+        <f>(C20^2)*((1/A20^2)*(1-F20^2)+1/B20*(E20)) / ((1-F20^2)*(1+E20-G20)-E20)</f>
+        <v>17.311128871128826</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2257,26 +2228,26 @@
         <v>1.25</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="D21">
         <v>0.2</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>1.6</v>
+        <v>1.44</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
-        <v>1.6</v>
+        <f t="shared" si="2"/>
+        <v>1.44</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
-        <v>-7.9094339622641456</v>
+        <f t="shared" si="0"/>
+        <v>-29.616692563818006</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2288,26 +2259,26 @@
         <v>1.25</v>
       </c>
       <c r="C22">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="D22">
         <v>0.2</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>1.6800000000000002</v>
+        <v>1.52</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
-        <v>1.6800000000000002</v>
+        <f t="shared" si="2"/>
+        <v>1.52</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
-        <v>-6.577145025135156</v>
+        <f t="shared" si="0"/>
+        <v>-11.170248030347238</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2319,26 +2290,26 @@
         <v>1.25</v>
       </c>
       <c r="C23">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="D23">
         <v>0.2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>1.7600000000000002</v>
+        <v>1.6</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
-        <v>1.7600000000000002</v>
+        <f t="shared" si="2"/>
+        <v>1.6</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
-        <v>-5.8719443167640648</v>
+        <f t="shared" si="0"/>
+        <v>-7.9094339622641456</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2350,26 +2321,26 @@
         <v>1.25</v>
       </c>
       <c r="C24">
-        <v>2.2999999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="D24">
         <v>0.2</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>1.8399999999999999</v>
+        <v>1.6800000000000002</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
-        <v>1.8399999999999999</v>
+        <f t="shared" si="2"/>
+        <v>1.6800000000000002</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
-        <v>-5.4494833823742228</v>
+        <f t="shared" si="0"/>
+        <v>-6.577145025135156</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2381,26 +2352,26 @@
         <v>1.25</v>
       </c>
       <c r="C25">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D25">
         <v>0.2</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>1.92</v>
+        <v>1.7600000000000002</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
-        <v>1.92</v>
+        <f t="shared" si="2"/>
+        <v>1.7600000000000002</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
-        <v>-5.1790471269882268</v>
+        <f t="shared" si="0"/>
+        <v>-5.8719443167640648</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2412,26 +2383,26 @@
         <v>1.25</v>
       </c>
       <c r="C26">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D26">
         <v>0.2</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1.8399999999999999</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1.8399999999999999</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
-        <v>-4.9999999999999991</v>
+        <f t="shared" si="0"/>
+        <v>-5.4494833823742228</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2443,26 +2414,26 @@
         <v>1.25</v>
       </c>
       <c r="C27">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="D27">
         <v>0.2</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>2.08</v>
+        <v>1.92</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
-        <v>2.08</v>
+        <f t="shared" si="2"/>
+        <v>1.92</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
-        <v>-4.8803097646258173</v>
+        <f t="shared" si="0"/>
+        <v>-5.1790471269882268</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2474,26 +2445,26 @@
         <v>1.25</v>
       </c>
       <c r="C28">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="D28">
         <v>0.2</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>2.16</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
-        <v>2.16</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
-        <v>-4.8014277174646631</v>
+        <f t="shared" si="0"/>
+        <v>-4.9999999999999991</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -2505,26 +2476,26 @@
         <v>1.25</v>
       </c>
       <c r="C29">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="D29">
         <v>0.2</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>2.2399999999999998</v>
+        <v>2.08</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>2.2399999999999998</v>
+        <f t="shared" si="2"/>
+        <v>2.08</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
-        <v>-4.7518514824407587</v>
+        <f t="shared" si="0"/>
+        <v>-4.8803097646258173</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -2536,26 +2507,26 @@
         <v>1.25</v>
       </c>
       <c r="C30">
-        <v>2.9</v>
+        <v>2.7</v>
       </c>
       <c r="D30">
         <v>0.2</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>2.3199999999999998</v>
+        <v>2.16</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
-        <v>2.3199999999999998</v>
+        <f t="shared" si="2"/>
+        <v>2.16</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
-        <v>-4.7240588850979384</v>
+        <f t="shared" si="0"/>
+        <v>-4.8014277174646631</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2567,26 +2538,26 @@
         <v>1.25</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="D31">
         <v>0.2</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>2.4</v>
+        <v>2.2399999999999998</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
-        <v>2.4</v>
+        <f t="shared" si="2"/>
+        <v>2.2399999999999998</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
-        <v>-4.7129172714078367</v>
+        <f t="shared" si="0"/>
+        <v>-4.7518514824407587</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2598,26 +2569,26 @@
         <v>1.25</v>
       </c>
       <c r="C32">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="D32">
         <v>0.2</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>2.48</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
-        <v>2.48</v>
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
-        <v>-4.7148007168387016</v>
+        <f t="shared" si="0"/>
+        <v>-4.7240588850979384</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2629,26 +2600,26 @@
         <v>1.25</v>
       </c>
       <c r="C33">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="D33">
         <v>0.2</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>2.56</v>
+        <v>2.4</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
-        <v>2.56</v>
+        <f t="shared" si="2"/>
+        <v>2.4</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
-        <v>-4.7270725656938435</v>
+        <f t="shared" si="0"/>
+        <v>-4.7129172714078367</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2660,26 +2631,26 @@
         <v>1.25</v>
       </c>
       <c r="C34">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="D34">
         <v>0.2</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>2.6399999999999997</v>
+        <v>2.48</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
-        <v>2.6399999999999997</v>
+        <f t="shared" si="2"/>
+        <v>2.48</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
-        <v>-4.7477680633580039</v>
+        <f t="shared" si="0"/>
+        <v>-4.7148007168387016</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2691,26 +2662,26 @@
         <v>1.25</v>
       </c>
       <c r="C35">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="D35">
         <v>0.2</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>2.7199999999999998</v>
+        <v>2.56</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
-        <v>2.7199999999999998</v>
+        <f t="shared" si="2"/>
+        <v>2.56</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
-        <v>-4.775392140395196</v>
+        <f t="shared" si="0"/>
+        <v>-4.7270725656938435</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2722,26 +2693,26 @@
         <v>1.25</v>
       </c>
       <c r="C36">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="D36">
         <v>0.2</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>2.8</v>
+        <v>2.6399999999999997</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
-        <v>2.8</v>
+        <f t="shared" si="2"/>
+        <v>2.6399999999999997</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
-        <v>-4.8087862993298582</v>
+        <f t="shared" si="0"/>
+        <v>-4.7477680633580039</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2753,26 +2724,26 @@
         <v>1.25</v>
       </c>
       <c r="C37">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="D37">
         <v>0.2</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>2.88</v>
+        <v>2.7199999999999998</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
-        <v>2.88</v>
+        <f t="shared" si="2"/>
+        <v>2.7199999999999998</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
-        <v>-4.8470384862465687</v>
+        <f t="shared" si="0"/>
+        <v>-4.775392140395196</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2784,26 +2755,26 @@
         <v>1.25</v>
       </c>
       <c r="C38">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
       <c r="D38">
         <v>0.2</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>2.96</v>
+        <v>2.8</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
-        <v>2.96</v>
+        <f t="shared" si="2"/>
+        <v>2.8</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
-        <v>-4.8894205468835441</v>
+        <f t="shared" si="0"/>
+        <v>-4.8087862993298582</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2815,26 +2786,26 @@
         <v>1.25</v>
       </c>
       <c r="C39">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="D39">
         <v>0.2</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>3.04</v>
+        <v>2.88</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
-        <v>3.04</v>
+        <f t="shared" si="2"/>
+        <v>2.88</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
-        <v>-4.9353438741601483</v>
+        <f t="shared" si="0"/>
+        <v>-4.8470384862465687</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2846,26 +2817,26 @@
         <v>1.25</v>
       </c>
       <c r="C40">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
       <c r="D40">
         <v>0.2</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>3.12</v>
+        <v>2.96</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
-        <v>3.12</v>
+        <f t="shared" si="2"/>
+        <v>2.96</v>
       </c>
       <c r="H40">
-        <f t="shared" si="2"/>
-        <v>-4.9843273453402173</v>
+        <f t="shared" si="0"/>
+        <v>-4.8894205468835441</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2877,26 +2848,26 @@
         <v>1.25</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="D41">
         <v>0.2</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>3.2</v>
+        <v>3.04</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
-        <v>3.2</v>
+        <f t="shared" si="2"/>
+        <v>3.04</v>
       </c>
       <c r="H41">
-        <f t="shared" si="2"/>
-        <v>-5.0359737417943107</v>
+        <f t="shared" si="0"/>
+        <v>-4.9353438741601483</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -2908,26 +2879,26 @@
         <v>1.25</v>
       </c>
       <c r="C42">
-        <v>4.0999999999999996</v>
+        <v>3.9</v>
       </c>
       <c r="D42">
         <v>0.2</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>3.28</v>
+        <v>3.12</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
-        <v>3.28</v>
+        <f t="shared" si="2"/>
+        <v>3.12</v>
       </c>
       <c r="H42">
-        <f t="shared" si="2"/>
-        <v>-5.0899521372638308</v>
+        <f t="shared" si="0"/>
+        <v>-4.9843273453402173</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2939,26 +2910,26 @@
         <v>1.25</v>
       </c>
       <c r="C43">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="D43">
         <v>0.2</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F43">
         <f t="shared" si="4"/>
-        <v>3.3600000000000003</v>
+        <v>3.2</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
-        <v>3.3600000000000003</v>
+        <f t="shared" si="2"/>
+        <v>3.2</v>
       </c>
       <c r="H43">
-        <f t="shared" si="2"/>
-        <v>-5.1459845590136819</v>
+        <f t="shared" si="0"/>
+        <v>-5.0359737417943107</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2970,26 +2941,26 @@
         <v>1.25</v>
       </c>
       <c r="C44">
-        <v>4.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D44">
         <v>0.2</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F44">
         <f t="shared" si="4"/>
-        <v>3.44</v>
+        <v>3.28</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
-        <v>3.44</v>
+        <f t="shared" si="2"/>
+        <v>3.28</v>
       </c>
       <c r="H44">
-        <f t="shared" si="2"/>
-        <v>-5.2038357563202853</v>
+        <f t="shared" si="0"/>
+        <v>-5.0899521372638308</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -3001,26 +2972,26 @@
         <v>1.25</v>
       </c>
       <c r="C45">
-        <v>4.4000000000000004</v>
+        <v>4.2</v>
       </c>
       <c r="D45">
         <v>0.2</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F45">
         <f t="shared" si="4"/>
-        <v>3.5200000000000005</v>
+        <v>3.3600000000000003</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
-        <v>3.5200000000000005</v>
+        <f t="shared" si="2"/>
+        <v>3.3600000000000003</v>
       </c>
       <c r="H45">
-        <f t="shared" si="2"/>
-        <v>-5.2633052611542377</v>
+        <f t="shared" si="0"/>
+        <v>-5.1459845590136819</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -3032,26 +3003,26 @@
         <v>1.25</v>
       </c>
       <c r="C46">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="D46">
         <v>0.2</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F46">
         <f t="shared" si="4"/>
-        <v>3.6</v>
+        <v>3.44</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
-        <v>3.6</v>
+        <f t="shared" si="2"/>
+        <v>3.44</v>
       </c>
       <c r="H46">
-        <f t="shared" si="2"/>
-        <v>-5.3242211619421829</v>
+        <f t="shared" si="0"/>
+        <v>-5.2038357563202853</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -3063,26 +3034,26 @@
         <v>1.25</v>
       </c>
       <c r="C47">
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D47">
         <v>0.2</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F47">
         <f t="shared" si="4"/>
-        <v>3.6799999999999997</v>
+        <v>3.5200000000000005</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
-        <v>3.6799999999999997</v>
+        <f t="shared" si="2"/>
+        <v>3.5200000000000005</v>
       </c>
       <c r="H47">
-        <f t="shared" si="2"/>
-        <v>-5.3864351730093416</v>
+        <f t="shared" si="0"/>
+        <v>-5.2633052611542377</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -3094,26 +3065,26 @@
         <v>1.25</v>
       </c>
       <c r="C48">
-        <v>4.7</v>
+        <v>4.5</v>
       </c>
       <c r="D48">
         <v>0.2</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F48">
         <f t="shared" si="4"/>
-        <v>3.7600000000000002</v>
+        <v>3.6</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
-        <v>3.7600000000000002</v>
+        <f t="shared" si="2"/>
+        <v>3.6</v>
       </c>
       <c r="H48">
-        <f t="shared" si="2"/>
-        <v>-5.4498186948556508</v>
+        <f t="shared" si="0"/>
+        <v>-5.3242211619421829</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -3125,26 +3096,26 @@
         <v>1.25</v>
       </c>
       <c r="C49">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D49">
         <v>0.2</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F49">
         <f t="shared" si="4"/>
-        <v>3.84</v>
+        <v>3.6799999999999997</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
-        <v>3.84</v>
+        <f t="shared" si="2"/>
+        <v>3.6799999999999997</v>
       </c>
       <c r="H49">
-        <f t="shared" si="2"/>
-        <v>-5.5142596398885591</v>
+        <f t="shared" si="0"/>
+        <v>-5.3864351730093416</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3156,26 +3127,26 @@
         <v>1.25</v>
       </c>
       <c r="C50">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
       <c r="D50">
         <v>0.2</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F50">
         <f t="shared" si="4"/>
-        <v>3.9200000000000004</v>
+        <v>3.7600000000000002</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
-        <v>3.9200000000000004</v>
+        <f t="shared" si="2"/>
+        <v>3.7600000000000002</v>
       </c>
       <c r="H50">
-        <f t="shared" si="2"/>
-        <v>-5.5796598550984688</v>
+        <f t="shared" si="0"/>
+        <v>-5.4498186948556508</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -3187,25 +3158,87 @@
         <v>1.25</v>
       </c>
       <c r="C51">
+        <v>4.8</v>
+      </c>
+      <c r="D51">
+        <v>0.2</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>3.84</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>3.84</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>-5.5142596398885591</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>1.25</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="C52">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D52">
+        <v>0.2</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="4"/>
+        <v>3.9200000000000004</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>3.9200000000000004</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>-5.5796598550984688</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>1.25</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="C53">
         <v>5</v>
       </c>
-      <c r="D51">
-        <v>0.2</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F51">
+      <c r="D53">
+        <v>0.2</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="F53">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G51">
-        <f t="shared" si="1"/>
+      <c r="G53">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="H51">
-        <f t="shared" si="2"/>
+      <c r="H53">
+        <f t="shared" si="0"/>
         <v>-5.6459330143540676</v>
       </c>
     </row>

</xml_diff>